<commit_message>
cleaned up function calls
to ensure aggregate_flows is called properly everywhere.

Also set up testing file for tomorrow.
</commit_message>
<xml_diff>
--- a/data/steel/factories/IBF-factory-BFG CCS.xlsx
+++ b/data/steel/factories/IBF-factory-BFG CCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A381DB7E-F2C5-2B4B-8936-927BC7E624C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C582A8-94B8-B549-A17D-C779DD054CB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="26520" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="26520" windowHeight="16520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chains" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="62">
   <si>
     <t>Inflow</t>
   </si>
@@ -129,9 +129,6 @@
     <t>o flowtype</t>
   </si>
   <si>
-    <t>fuel</t>
-  </si>
-  <si>
     <t>process_ID</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>simple_oxygen</t>
   </si>
   <si>
-    <t>simple_fuel</t>
-  </si>
-  <si>
     <t>simple_pellets</t>
   </si>
   <si>
@@ -216,13 +210,10 @@
     <t>CO2 Storage</t>
   </si>
   <si>
-    <t>secondary fuel</t>
-  </si>
-  <si>
-    <t>secondary biofuel</t>
-  </si>
-  <si>
-    <t>biofuel</t>
+    <t>simple_casting</t>
+  </si>
+  <si>
+    <t>hot rolled coil</t>
   </si>
 </sst>
 </file>
@@ -638,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -693,21 +684,21 @@
         <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -721,7 +712,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -735,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -749,63 +740,49 @@
         <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -815,10 +792,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,25 +857,25 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -906,13 +883,13 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -921,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -932,22 +909,22 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
         <v>29</v>
@@ -955,25 +932,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
         <v>29</v>
@@ -999,7 +976,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
         <v>9</v>
@@ -1007,7 +984,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>22</v>
@@ -1022,10 +999,10 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
         <v>9</v>
@@ -1051,7 +1028,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" t="s">
         <v>21</v>
@@ -1077,7 +1054,7 @@
         <v>19</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
         <v>24</v>
@@ -1103,7 +1080,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I10" t="s">
         <v>24</v>
@@ -1129,7 +1106,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
         <v>24</v>
@@ -1155,7 +1132,7 @@
         <v>19</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I12" t="s">
         <v>24</v>
@@ -1163,7 +1140,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>22</v>
@@ -1181,7 +1158,7 @@
         <v>19</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I13" t="s">
         <v>24</v>
@@ -1192,33 +1169,33 @@
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="I14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1233,7 +1210,7 @@
         <v>19</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I15" t="s">
         <v>24</v>
@@ -1244,293 +1221,85 @@
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
       </c>
       <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>19</v>
       </c>
       <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="H27" s="1"/>
-      <c r="I27" s="6"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1541,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1557,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1568,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1579,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -1590,16 +1359,22 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -1625,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1633,24 +1408,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>